<commit_message>
added a bunch of stuff, trying to make a website out of this
</commit_message>
<xml_diff>
--- a/sortedByRCGroup.xlsx
+++ b/sortedByRCGroup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mannb\source\repos\recruitment_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AA0CD8-911E-45D6-AA64-949E8D8E438B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A2104F-784A-4873-B063-59F29ADAAE7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12771" yWindow="0" windowWidth="13029" windowHeight="16509" tabRatio="833" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7197,7 +7197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -7209,7 +7209,6 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7514,8 +7513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A356F6-E45F-4ABA-99ED-5DC1C3A16524}">
   <dimension ref="A1:HH519"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A380" zoomScale="211" workbookViewId="0">
-      <selection activeCell="A387" sqref="A387:XFD387"/>
+    <sheetView tabSelected="1" topLeftCell="A284" zoomScale="211" workbookViewId="0">
+      <selection activeCell="B300" sqref="B300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -9400,238 +9399,30 @@
       </c>
     </row>
     <row r="33" spans="1:216" s="3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A33">
+      <c r="A33" s="3">
         <v>9714792</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="3">
         <v>32</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="3" t="s">
         <v>1012</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="3" t="s">
         <v>1013</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="3" t="s">
         <v>1014</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" s="3" t="s">
         <v>1015</v>
       </c>
-      <c r="G33" s="4">
+      <c r="G33" s="5">
         <v>45792.493750000001</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="3">
         <v>5</v>
       </c>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
-      <c r="M33" s="6"/>
-      <c r="N33" s="6"/>
-      <c r="O33" s="6"/>
-      <c r="P33" s="6"/>
-      <c r="Q33" s="6"/>
-      <c r="R33" s="6"/>
-      <c r="S33" s="6"/>
-      <c r="T33" s="6"/>
-      <c r="U33" s="6"/>
-      <c r="V33" s="6"/>
-      <c r="W33" s="6"/>
-      <c r="X33" s="6"/>
-      <c r="Y33" s="6"/>
-      <c r="Z33" s="6"/>
-      <c r="AA33" s="6"/>
-      <c r="AB33" s="6"/>
-      <c r="AC33" s="6"/>
-      <c r="AD33" s="6"/>
-      <c r="AE33" s="6"/>
-      <c r="AF33" s="6"/>
-      <c r="AG33" s="6"/>
-      <c r="AH33" s="6"/>
-      <c r="AI33" s="6"/>
-      <c r="AJ33" s="6"/>
-      <c r="AK33" s="6"/>
-      <c r="AL33" s="6"/>
-      <c r="AM33" s="6"/>
-      <c r="AN33" s="6"/>
-      <c r="AO33" s="6"/>
-      <c r="AP33" s="6"/>
-      <c r="AQ33" s="6"/>
-      <c r="AR33" s="6"/>
-      <c r="AS33" s="6"/>
-      <c r="AT33" s="6"/>
-      <c r="AU33" s="6"/>
-      <c r="AV33" s="6"/>
-      <c r="AW33" s="6"/>
-      <c r="AX33" s="6"/>
-      <c r="AY33" s="6"/>
-      <c r="AZ33" s="6"/>
-      <c r="BA33" s="6"/>
-      <c r="BB33" s="6"/>
-      <c r="BC33" s="6"/>
-      <c r="BD33" s="6"/>
-      <c r="BE33" s="6"/>
-      <c r="BF33" s="6"/>
-      <c r="BG33" s="6"/>
-      <c r="BH33" s="6"/>
-      <c r="BI33" s="6"/>
-      <c r="BJ33" s="6"/>
-      <c r="BK33" s="6"/>
-      <c r="BL33" s="6"/>
-      <c r="BM33" s="6"/>
-      <c r="BN33" s="6"/>
-      <c r="BO33" s="6"/>
-      <c r="BP33" s="6"/>
-      <c r="BQ33" s="6"/>
-      <c r="BR33" s="6"/>
-      <c r="BS33" s="6"/>
-      <c r="BT33" s="6"/>
-      <c r="BU33" s="6"/>
-      <c r="BV33" s="6"/>
-      <c r="BW33" s="6"/>
-      <c r="BX33" s="6"/>
-      <c r="BY33" s="6"/>
-      <c r="BZ33" s="6"/>
-      <c r="CA33" s="6"/>
-      <c r="CB33" s="6"/>
-      <c r="CC33" s="6"/>
-      <c r="CD33" s="6"/>
-      <c r="CE33" s="6"/>
-      <c r="CF33" s="6"/>
-      <c r="CG33" s="6"/>
-      <c r="CH33" s="6"/>
-      <c r="CI33" s="6"/>
-      <c r="CJ33" s="6"/>
-      <c r="CK33" s="6"/>
-      <c r="CL33" s="6"/>
-      <c r="CM33" s="6"/>
-      <c r="CN33" s="6"/>
-      <c r="CO33" s="6"/>
-      <c r="CP33" s="6"/>
-      <c r="CQ33" s="6"/>
-      <c r="CR33" s="6"/>
-      <c r="CS33" s="6"/>
-      <c r="CT33" s="6"/>
-      <c r="CU33" s="6"/>
-      <c r="CV33" s="6"/>
-      <c r="CW33" s="6"/>
-      <c r="CX33" s="6"/>
-      <c r="CY33" s="6"/>
-      <c r="CZ33" s="6"/>
-      <c r="DA33" s="6"/>
-      <c r="DB33" s="6"/>
-      <c r="DC33" s="6"/>
-      <c r="DD33" s="6"/>
-      <c r="DE33" s="6"/>
-      <c r="DF33" s="6"/>
-      <c r="DG33" s="6"/>
-      <c r="DH33" s="6"/>
-      <c r="DI33" s="6"/>
-      <c r="DJ33" s="6"/>
-      <c r="DK33" s="6"/>
-      <c r="DL33" s="6"/>
-      <c r="DM33" s="6"/>
-      <c r="DN33" s="6"/>
-      <c r="DO33" s="6"/>
-      <c r="DP33" s="6"/>
-      <c r="DQ33" s="6"/>
-      <c r="DR33" s="6"/>
-      <c r="DS33" s="6"/>
-      <c r="DT33" s="6"/>
-      <c r="DU33" s="6"/>
-      <c r="DV33" s="6"/>
-      <c r="DW33" s="6"/>
-      <c r="DX33" s="6"/>
-      <c r="DY33" s="6"/>
-      <c r="DZ33" s="6"/>
-      <c r="EA33" s="6"/>
-      <c r="EB33" s="6"/>
-      <c r="EC33" s="6"/>
-      <c r="ED33" s="6"/>
-      <c r="EE33" s="6"/>
-      <c r="EF33" s="6"/>
-      <c r="EG33" s="6"/>
-      <c r="EH33" s="6"/>
-      <c r="EI33" s="6"/>
-      <c r="EJ33" s="6"/>
-      <c r="EK33" s="6"/>
-      <c r="EL33" s="6"/>
-      <c r="EM33" s="6"/>
-      <c r="EN33" s="6"/>
-      <c r="EO33" s="6"/>
-      <c r="EP33" s="6"/>
-      <c r="EQ33" s="6"/>
-      <c r="ER33" s="6"/>
-      <c r="ES33" s="6"/>
-      <c r="ET33" s="6"/>
-      <c r="EU33" s="6"/>
-      <c r="EV33" s="6"/>
-      <c r="EW33" s="6"/>
-      <c r="EX33" s="6"/>
-      <c r="EY33" s="6"/>
-      <c r="EZ33" s="6"/>
-      <c r="FA33" s="6"/>
-      <c r="FB33" s="6"/>
-      <c r="FC33" s="6"/>
-      <c r="FD33" s="6"/>
-      <c r="FE33" s="6"/>
-      <c r="FF33" s="6"/>
-      <c r="FG33" s="6"/>
-      <c r="FH33" s="6"/>
-      <c r="FI33" s="6"/>
-      <c r="FJ33" s="6"/>
-      <c r="FK33" s="6"/>
-      <c r="FL33" s="6"/>
-      <c r="FM33" s="6"/>
-      <c r="FN33" s="6"/>
-      <c r="FO33" s="6"/>
-      <c r="FP33" s="6"/>
-      <c r="FQ33" s="6"/>
-      <c r="FR33" s="6"/>
-      <c r="FS33" s="6"/>
-      <c r="FT33" s="6"/>
-      <c r="FU33" s="6"/>
-      <c r="FV33" s="6"/>
-      <c r="FW33" s="6"/>
-      <c r="FX33" s="6"/>
-      <c r="FY33" s="6"/>
-      <c r="FZ33" s="6"/>
-      <c r="GA33" s="6"/>
-      <c r="GB33" s="6"/>
-      <c r="GC33" s="6"/>
-      <c r="GD33" s="6"/>
-      <c r="GE33" s="6"/>
-      <c r="GF33" s="6"/>
-      <c r="GG33" s="6"/>
-      <c r="GH33" s="6"/>
-      <c r="GI33" s="6"/>
-      <c r="GJ33" s="6"/>
-      <c r="GK33" s="6"/>
-      <c r="GL33" s="6"/>
-      <c r="GM33" s="6"/>
-      <c r="GN33" s="6"/>
-      <c r="GO33" s="6"/>
-      <c r="GP33" s="6"/>
-      <c r="GQ33" s="6"/>
-      <c r="GR33" s="6"/>
-      <c r="GS33" s="6"/>
-      <c r="GT33" s="6"/>
-      <c r="GU33" s="6"/>
-      <c r="GV33" s="6"/>
-      <c r="GW33" s="6"/>
-      <c r="GX33" s="6"/>
-      <c r="GY33" s="6"/>
-      <c r="GZ33" s="6"/>
-      <c r="HA33" s="6"/>
-      <c r="HB33" s="6"/>
-      <c r="HC33" s="6"/>
-      <c r="HD33" s="6"/>
-      <c r="HE33" s="6"/>
-      <c r="HF33" s="6"/>
-      <c r="HG33" s="6"/>
-      <c r="HH33" s="6"/>
     </row>
     <row r="34" spans="1:216" x14ac:dyDescent="0.4">
       <c r="A34">
@@ -12074,29 +11865,29 @@
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="1:216" x14ac:dyDescent="0.4">
-      <c r="A72">
+    <row r="72" spans="1:216" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A72" s="3">
         <v>9727644</v>
       </c>
-      <c r="B72">
+      <c r="B72" s="3">
         <v>74</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" s="3" t="s">
         <v>1018</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D72" s="3" t="s">
         <v>1019</v>
       </c>
-      <c r="E72" t="s">
+      <c r="E72" s="3" t="s">
         <v>1020</v>
       </c>
-      <c r="F72" t="s">
+      <c r="F72" s="3" t="s">
         <v>1021</v>
       </c>
-      <c r="G72" s="4">
+      <c r="G72" s="5">
         <v>45812.854166666664</v>
       </c>
-      <c r="H72">
+      <c r="H72" s="3">
         <v>5</v>
       </c>
     </row>
@@ -16777,55 +16568,55 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:216" x14ac:dyDescent="0.4">
-      <c r="A149">
+    <row r="149" spans="1:216" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A149" s="3">
         <v>9767166</v>
       </c>
-      <c r="B149">
+      <c r="B149" s="3">
         <v>152</v>
       </c>
-      <c r="C149" t="s">
+      <c r="C149" s="3" t="s">
         <v>1026</v>
       </c>
-      <c r="D149" t="s">
+      <c r="D149" s="3" t="s">
         <v>1409</v>
       </c>
-      <c r="E149" t="s">
+      <c r="E149" s="3" t="s">
         <v>1410</v>
       </c>
-      <c r="F149" t="s">
+      <c r="F149" s="3" t="s">
         <v>1411</v>
       </c>
-      <c r="G149" s="4">
+      <c r="G149" s="5">
         <v>45847.59097222222</v>
       </c>
-      <c r="H149">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="150" spans="1:216" s="6" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A150" s="6">
+      <c r="H149" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="150" spans="1:216" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A150" s="3">
         <v>9767196</v>
       </c>
-      <c r="B150" s="6">
+      <c r="B150" s="3">
         <v>153</v>
       </c>
-      <c r="C150" s="6" t="s">
+      <c r="C150" s="3" t="s">
         <v>1314</v>
       </c>
-      <c r="D150" s="6" t="s">
+      <c r="D150" s="3" t="s">
         <v>1672</v>
       </c>
-      <c r="E150" s="6" t="s">
+      <c r="E150" s="3" t="s">
         <v>1673</v>
       </c>
-      <c r="F150" s="6" t="s">
+      <c r="F150" s="3" t="s">
         <v>1674</v>
       </c>
-      <c r="G150" s="7">
+      <c r="G150" s="5">
         <v>45847.609027777777</v>
       </c>
-      <c r="H150" s="6">
+      <c r="H150" s="3">
         <v>12</v>
       </c>
     </row>
@@ -27784,55 +27575,55 @@
         <v>18</v>
       </c>
     </row>
-    <row r="389" spans="1:216" x14ac:dyDescent="0.4">
-      <c r="A389">
+    <row r="389" spans="1:216" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A389" s="3">
         <v>10077258</v>
       </c>
-      <c r="B389">
+      <c r="B389" s="3">
         <v>409</v>
       </c>
-      <c r="C389" t="s">
+      <c r="C389" s="3" t="s">
         <v>945</v>
       </c>
-      <c r="D389" t="s">
+      <c r="D389" s="3" t="s">
         <v>1749</v>
       </c>
-      <c r="E389" t="s">
+      <c r="E389" s="3" t="s">
         <v>2011</v>
       </c>
-      <c r="F389" t="s">
+      <c r="F389" s="3" t="s">
         <v>2012</v>
       </c>
-      <c r="G389" s="4">
+      <c r="G389" s="5">
         <v>45921.751388888886</v>
       </c>
-      <c r="H389">
+      <c r="H389" s="3">
         <v>16</v>
       </c>
     </row>
-    <row r="390" spans="1:216" x14ac:dyDescent="0.4">
-      <c r="A390">
+    <row r="390" spans="1:216" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A390" s="3">
         <v>10077461</v>
       </c>
-      <c r="B390">
+      <c r="B390" s="3">
         <v>410</v>
       </c>
-      <c r="C390" t="s">
+      <c r="C390" s="3" t="s">
         <v>1026</v>
       </c>
-      <c r="D390" t="s">
+      <c r="D390" s="3" t="s">
         <v>1823</v>
       </c>
-      <c r="E390" t="s">
+      <c r="E390" s="3" t="s">
         <v>1824</v>
       </c>
-      <c r="F390" t="s">
+      <c r="F390" s="3" t="s">
         <v>1825</v>
       </c>
-      <c r="G390" s="4">
+      <c r="G390" s="5">
         <v>45921.987500000003</v>
       </c>
-      <c r="H390">
+      <c r="H390" s="3">
         <v>14</v>
       </c>
     </row>

</xml_diff>